<commit_message>
Replacing HTML file with new runs.
</commit_message>
<xml_diff>
--- a/example/tri.xlsx
+++ b/example/tri.xlsx
@@ -468,21 +468,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>52.7 (48.7+4.16,-5.15)</t>
+          <t>46.0 (36.3+6.36,-8.09)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>177.0 (161.0+22.5,-27.6)</t>
+          <t>207.0 (115.0+41.1,-28.8)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>59.2 (64.2+11.6,-12.4)</t>
+          <t>48.0 (83.5+19.3,-27.7)</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>8.449999999999999</v>
+        <v>9.869999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>